<commit_message>
Monitoreo CRGs - Incorporacion de Importe CRG al monitoreo de CRGs facturados. Falta hacer el group by de este campo
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FACOEP\DBA\Reportes BI\2021\Monitoreo CRGs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Monitoreo CRGs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Parametros servidor</t>
   </si>
@@ -74,13 +74,10 @@
     <t>user_server</t>
   </si>
   <si>
-    <t>openpg</t>
-  </si>
-  <si>
-    <t>openpgpwd</t>
-  </si>
-  <si>
-    <t>C:/Users/User/Desktop/FACOEP/DBA/Reportes BI/2021/Monitoreo CRGs</t>
+    <t>C:/Users/iachenbach/Gobierno de la Ciudad de Buenos Aires/Pablo Alfredo Gadea - Tablero Facoep P BI/FACOEP/DBA/Reportes BI/2021/Monitoreo CRGs/</t>
+  </si>
+  <si>
+    <t>odoo</t>
   </si>
 </sst>
 </file>
@@ -413,7 +410,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -471,7 +468,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Monitoreo CRGs - Implementacion Solapa CRGs facturados con rango de fecha y tabla de detalle
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>Parametros servidor</t>
   </si>
@@ -68,16 +68,10 @@
     <t>E:/Personales/Sistemas/Agustin/Reportes BI/2021/Cobranzas/Versión 7</t>
   </si>
   <si>
-    <t>host_server</t>
-  </si>
-  <si>
-    <t>user_server</t>
-  </si>
-  <si>
-    <t>C:/Users/iachenbach/Gobierno de la Ciudad de Buenos Aires/Pablo Alfredo Gadea - Tablero Facoep P BI/FACOEP/DBA/Reportes BI/2021/Monitoreo CRGs/</t>
-  </si>
-  <si>
     <t>odoo</t>
+  </si>
+  <si>
+    <t>C:/Users/iachenbach/Gobierno de la Ciudad de Buenos Aires/Pablo Alfredo Gadea - Tablero Facoep P BI/FACOEP/DBA/Reportes BI/2021/Monitoreo CRGs</t>
   </si>
 </sst>
 </file>
@@ -410,13 +404,13 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="88.5703125" customWidth="1"/>
+    <col min="2" max="2" width="135.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -446,7 +440,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -457,7 +451,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -468,7 +462,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -476,7 +470,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -487,7 +481,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Monitoreo CRGs con database suministrado archivo parametros
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>Parametros servidor</t>
   </si>
@@ -65,26 +65,47 @@
     <t>facoep2017</t>
   </si>
   <si>
-    <t>E:/Personales/Sistemas/Agustin/Reportes BI/2021/Cobranzas/Versión 7</t>
-  </si>
-  <si>
     <t>odoo</t>
   </si>
   <si>
     <t>C:/Users/iachenbach/Gobierno de la Ciudad de Buenos Aires/Pablo Alfredo Gadea - Tablero Facoep P BI/FACOEP/DBA/Reportes BI/2021/Monitoreo CRGs</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facoep </t>
+  </si>
+  <si>
+    <t>Facoep</t>
+  </si>
+  <si>
+    <t>E:/Personales/Sistemas/Agustin/Reportes BI/2021/MonitoreoCRGs</t>
+  </si>
+  <si>
+    <t>10.22.0.142</t>
+  </si>
+  <si>
+    <t>serveradmin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -107,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,8 +149,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0">
-  <autoFilter ref="A1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Parametros servidor"/>
     <tableColumn id="2" name="Valor"/>
@@ -401,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +462,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -451,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -462,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -470,21 +492,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -492,10 +514,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -503,19 +525,75 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Incorporacion de campo Obra social
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
+++ b/DBA/Reportes BI/2021/Monitoreo CRGs/parametros_servidor.xlsx
@@ -74,9 +74,6 @@
     <t>database</t>
   </si>
   <si>
-    <t xml:space="preserve">facoep </t>
-  </si>
-  <si>
     <t>Facoep</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>serveradmin</t>
+  </si>
+  <si>
+    <t>facoep</t>
   </si>
 </sst>
 </file>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -561,7 +561,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -583,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>

</xml_diff>